<commit_message>
Added more accurate pricing
</commit_message>
<xml_diff>
--- a/GoPack v2.0 - Pi 3 Simulink r2017b/GoPack Board Rev A/GoPack2 Parts List.xlsx
+++ b/GoPack v2.0 - Pi 3 Simulink r2017b/GoPack Board Rev A/GoPack2 Parts List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm_000\Desktop\RaspberryPIC Git\raspberry-pic-gopack\GoPack Board Rev A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8281F59B-693A-48DD-871D-C3EE1535048F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D526418E-E63F-47E0-9493-C3DC085D2409}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="300" windowWidth="20736" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,7 +478,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,19 +502,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF222222"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -531,19 +518,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="6" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="6" tint="-0.499984740745262"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -553,12 +527,6 @@
       <sz val="10"/>
       <color theme="4" tint="-0.249977111117893"/>
       <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -715,15 +683,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -735,8 +702,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -745,33 +710,15 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1116,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1126,7 +1073,7 @@
     <col min="2" max="2" width="18.88671875" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="7" customWidth="1"/>
     <col min="6" max="6" width="12.5546875" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
@@ -1134,106 +1081,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="47">
-        <v>1</v>
-      </c>
-      <c r="F3" s="48">
+      <c r="D3" s="28"/>
+      <c r="E3" s="30">
+        <v>1</v>
+      </c>
+      <c r="F3" s="31">
         <v>66.349999999999994</v>
       </c>
-      <c r="G3" s="49">
+      <c r="G3" s="32">
         <f>F3/3</f>
         <v>22.116666666666664</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="50" t="s">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>3</v>
       </c>
-      <c r="F4" s="23">
-        <v>2.98</v>
-      </c>
-      <c r="G4" s="22">
+      <c r="F4" s="20">
+        <v>2.19</v>
+      </c>
+      <c r="G4" s="19">
         <f t="shared" ref="G4:G36" si="0">F4*E4</f>
-        <v>8.94</v>
+        <v>6.57</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="14">
-        <v>1</v>
-      </c>
-      <c r="F5" s="23">
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="20">
         <v>0.85099999999999998</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="19">
         <f t="shared" si="0"/>
         <v>0.85099999999999998</v>
       </c>
@@ -1242,22 +1189,22 @@
       <c r="A6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="14">
-        <v>1</v>
-      </c>
-      <c r="F6" s="23">
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="20">
         <v>0.85099999999999998</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="19">
         <f t="shared" si="0"/>
         <v>0.85099999999999998</v>
       </c>
@@ -1266,22 +1213,22 @@
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="14">
-        <v>1</v>
-      </c>
-      <c r="F7" s="23">
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="20">
         <v>5.13</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="19">
         <f t="shared" si="0"/>
         <v>5.13</v>
       </c>
@@ -1290,22 +1237,22 @@
       <c r="A8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="13">
-        <v>1</v>
-      </c>
-      <c r="F8" s="24">
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="21">
         <v>2.3340000000000001</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="19">
         <f t="shared" si="0"/>
         <v>2.3340000000000001</v>
       </c>
@@ -1314,22 +1261,22 @@
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="18" t="s">
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="14">
-        <v>1</v>
-      </c>
-      <c r="F9" s="23">
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+      <c r="F9" s="20">
         <v>0.92700000000000005</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="19">
         <f t="shared" si="0"/>
         <v>0.92700000000000005</v>
       </c>
@@ -1338,22 +1285,22 @@
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="23">
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="20">
         <v>0.92700000000000005</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="19">
         <f t="shared" si="0"/>
         <v>0.92700000000000005</v>
       </c>
@@ -1362,22 +1309,22 @@
       <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="18" t="s">
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="14">
-        <v>1</v>
-      </c>
-      <c r="F11" s="23">
+      <c r="E11" s="13">
+        <v>1</v>
+      </c>
+      <c r="F11" s="20">
         <v>0.93</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="19">
         <f t="shared" si="0"/>
         <v>0.93</v>
       </c>
@@ -1386,22 +1333,22 @@
       <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="14">
-        <v>1</v>
-      </c>
-      <c r="F12" s="23">
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20">
         <v>0.33900000000000002</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="19">
         <f t="shared" si="0"/>
         <v>0.33900000000000002</v>
       </c>
@@ -1410,22 +1357,22 @@
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="18" t="s">
+      <c r="B13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="14">
-        <v>1</v>
-      </c>
-      <c r="F13" s="23">
+      <c r="E13" s="13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="20">
         <v>0.21099999999999999</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="19">
         <f t="shared" si="0"/>
         <v>0.21099999999999999</v>
       </c>
@@ -1434,22 +1381,22 @@
       <c r="A14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="23">
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="20">
         <v>0.19500000000000001</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="19">
         <f t="shared" si="0"/>
         <v>0.19500000000000001</v>
       </c>
@@ -1458,22 +1405,22 @@
       <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="16">
-        <v>1</v>
-      </c>
-      <c r="F15" s="25">
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="22">
         <v>0.42399999999999999</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="19">
         <f t="shared" si="0"/>
         <v>0.42399999999999999</v>
       </c>
@@ -1482,22 +1429,22 @@
       <c r="A16" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="21" t="s">
+      <c r="B16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>5</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="20">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="19">
         <f t="shared" si="0"/>
         <v>4.1000000000000002E-2</v>
       </c>
@@ -1506,22 +1453,22 @@
       <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="18" t="s">
+      <c r="B17" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>3</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="20">
         <v>5.7599999999999998E-2</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="19">
         <f t="shared" si="0"/>
         <v>0.17280000000000001</v>
       </c>
@@ -1530,22 +1477,22 @@
       <c r="A18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="16">
-        <v>1</v>
-      </c>
-      <c r="F18" s="25">
+      <c r="E18" s="15">
+        <v>1</v>
+      </c>
+      <c r="F18" s="22">
         <v>2.1399999999999999E-2</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="19">
         <f t="shared" si="0"/>
         <v>2.1399999999999999E-2</v>
       </c>
@@ -1554,739 +1501,739 @@
       <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="15">
         <v>3</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="22">
         <v>7.5600000000000001E-2</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="19">
         <f t="shared" si="0"/>
         <v>0.2268</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="18" t="s">
+      <c r="B20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="15">
         <v>2</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="22">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="19">
         <f t="shared" si="0"/>
         <v>0.158</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="18" t="s">
+      <c r="B21" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="16">
-        <v>1</v>
-      </c>
-      <c r="F21" s="25">
+      <c r="E21" s="15">
+        <v>1</v>
+      </c>
+      <c r="F21" s="22">
         <v>0.71899999999999997</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="19">
         <f t="shared" si="0"/>
         <v>0.71899999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="18" t="s">
+      <c r="B22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="15">
         <v>2</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="22">
         <v>1.24</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="19">
         <f t="shared" si="0"/>
         <v>2.48</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="18" t="s">
+      <c r="B23" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="15">
         <v>2</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="22">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="19">
         <f t="shared" si="0"/>
         <v>8.8000000000000005E-3</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="15">
         <v>2</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="22">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="19">
         <f t="shared" si="0"/>
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="18" t="s">
+      <c r="B25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="16">
-        <v>1</v>
-      </c>
-      <c r="F25" s="25">
+      <c r="E25" s="15">
+        <v>1</v>
+      </c>
+      <c r="F25" s="22">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="19">
         <f t="shared" si="0"/>
         <v>5.1999999999999998E-3</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="18" t="s">
+      <c r="B26" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E26" s="16">
-        <v>1</v>
-      </c>
-      <c r="F26" s="25">
+      <c r="E26" s="15">
+        <v>1</v>
+      </c>
+      <c r="F26" s="22">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="19">
         <f t="shared" si="0"/>
         <v>5.1999999999999998E-3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="16">
-        <v>1</v>
-      </c>
-      <c r="F27" s="25">
+      <c r="E27" s="15">
+        <v>1</v>
+      </c>
+      <c r="F27" s="22">
         <v>0.27600000000000002</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>0.27600000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="9" t="s">
+      <c r="B28" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E28" s="16">
-        <v>1</v>
-      </c>
-      <c r="F28" s="25">
+      <c r="E28" s="15">
+        <v>1</v>
+      </c>
+      <c r="F28" s="22">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="18" t="s">
+      <c r="B29" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="16">
-        <v>1</v>
-      </c>
-      <c r="F29" s="25">
+      <c r="E29" s="15">
+        <v>1</v>
+      </c>
+      <c r="F29" s="22">
         <v>1.09E-2</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>1.09E-2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="18" t="s">
+      <c r="B30" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="16">
-        <v>1</v>
-      </c>
-      <c r="F30" s="25">
+      <c r="E30" s="15">
+        <v>1</v>
+      </c>
+      <c r="F30" s="22">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G30" s="19">
         <f t="shared" si="0"/>
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="18" t="s">
+      <c r="B31" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="13">
         <v>6</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="22">
         <v>1.1388</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>6.8328000000000007</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="21" t="s">
+      <c r="B32" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="14">
-        <v>1</v>
-      </c>
-      <c r="F32" s="23">
+      <c r="E32" s="13">
+        <v>1</v>
+      </c>
+      <c r="F32" s="20">
         <v>1.3160000000000001</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G32" s="19">
         <f t="shared" si="0"/>
         <v>1.3160000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="21" t="s">
+      <c r="B33" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="14">
-        <v>1</v>
-      </c>
-      <c r="F33" s="23">
+      <c r="E33" s="13">
+        <v>1</v>
+      </c>
+      <c r="F33" s="20">
         <v>0.74</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="19">
         <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="21" t="s">
+      <c r="B34" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="14">
-        <v>1</v>
-      </c>
-      <c r="F34" s="23">
+      <c r="E34" s="15">
+        <v>1</v>
+      </c>
+      <c r="F34" s="22">
         <v>2.73</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>2.73</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="20" t="s">
+      <c r="B35" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="14">
-        <v>1</v>
-      </c>
-      <c r="F35" s="23">
+      <c r="E35" s="15">
+        <v>1</v>
+      </c>
+      <c r="F35" s="22">
         <v>1.6</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="J35" s="27"/>
+      <c r="J35" s="24"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="18" t="s">
+      <c r="B36" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="15">
         <v>2</v>
       </c>
-      <c r="F36" s="25">
+      <c r="F36" s="22">
         <v>0.27300000000000002</v>
       </c>
-      <c r="G36" s="22">
+      <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0.54600000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="32" t="s">
+      <c r="B37" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E37" s="33">
+      <c r="E37" s="15">
         <v>3</v>
       </c>
-      <c r="F37" s="34">
-        <v>0.12</v>
-      </c>
-      <c r="G37" s="35">
+      <c r="F37" s="22">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="G37" s="19">
         <f>E37*F37</f>
-        <v>0.36</v>
+        <v>0.1278</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B38" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="37" t="s">
+      <c r="B38" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="15">
         <v>6</v>
       </c>
-      <c r="F38" s="39">
-        <v>0.13</v>
-      </c>
-      <c r="G38" s="35">
+      <c r="F38" s="22">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G38" s="19">
         <f t="shared" ref="G38:G44" si="1">E38*F38</f>
-        <v>0.78</v>
-      </c>
-      <c r="H38" s="9"/>
+        <v>0.03</v>
+      </c>
+      <c r="H38" s="8"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B39" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="40" t="s">
+      <c r="B39" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E39" s="38">
+      <c r="E39" s="15">
         <v>3</v>
       </c>
-      <c r="F39" s="39">
-        <v>0.38</v>
-      </c>
-      <c r="G39" s="35">
+      <c r="F39" s="22">
+        <v>0.159</v>
+      </c>
+      <c r="G39" s="19">
         <f t="shared" si="1"/>
-        <v>1.1400000000000001</v>
-      </c>
-      <c r="H39" s="9"/>
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="H39" s="8"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B40" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="37" t="s">
+      <c r="B40" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E40" s="38">
+      <c r="E40" s="15">
         <v>3</v>
       </c>
-      <c r="F40" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="G40" s="35">
+      <c r="F40" s="22">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G40" s="19">
         <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="H40" s="9"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B41" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="37" t="s">
+      <c r="B41" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D41" s="36" t="s">
+      <c r="D41" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E41" s="38">
-        <v>1</v>
-      </c>
-      <c r="F41" s="39">
-        <v>0.37</v>
-      </c>
-      <c r="G41" s="35">
+      <c r="E41" s="15">
+        <v>1</v>
+      </c>
+      <c r="F41" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="G41" s="19">
         <f t="shared" si="1"/>
-        <v>0.37</v>
-      </c>
-      <c r="H41" s="9"/>
+        <v>0.2</v>
+      </c>
+      <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B42" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="42" t="s">
+      <c r="B42" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="36" t="s">
+      <c r="D42" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E42" s="43">
-        <v>1</v>
-      </c>
-      <c r="F42" s="39">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="G42" s="35">
+      <c r="E42" s="13">
+        <v>1</v>
+      </c>
+      <c r="F42" s="22">
+        <v>1.58</v>
+      </c>
+      <c r="G42" s="19">
         <f t="shared" si="1"/>
-        <v>2.5499999999999998</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="38" t="s">
+      <c r="A43" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B43" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="37" t="s">
+      <c r="B43" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="D43" s="36" t="s">
+      <c r="D43" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E43" s="38">
+      <c r="E43" s="13">
         <v>3</v>
       </c>
-      <c r="F43" s="39">
-        <v>1.98</v>
-      </c>
-      <c r="G43" s="35">
+      <c r="F43" s="20">
+        <v>1.28</v>
+      </c>
+      <c r="G43" s="19">
         <f t="shared" si="1"/>
-        <v>5.9399999999999995</v>
+        <v>3.84</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="37" t="s">
+      <c r="B44" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D44" s="36" t="s">
+      <c r="D44" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="E44" s="33">
+      <c r="E44" s="13">
         <v>2</v>
       </c>
-      <c r="F44" s="39">
-        <v>0.71</v>
-      </c>
-      <c r="G44" s="35">
+      <c r="F44" s="20">
+        <v>0.33</v>
+      </c>
+      <c r="G44" s="19">
         <f t="shared" si="1"/>
-        <v>1.42</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B45" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="40">
+      <c r="B45" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="17">
         <v>1792902</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D45" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="E45" s="38">
-        <v>1</v>
-      </c>
-      <c r="F45" s="34">
-        <v>0.99</v>
-      </c>
-      <c r="G45" s="35">
+      <c r="E45" s="15">
+        <v>1</v>
+      </c>
+      <c r="F45" s="22">
+        <v>0.86</v>
+      </c>
+      <c r="G45" s="19">
         <f>E45*F45</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="30" t="s">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B46" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="37">
+      <c r="B46" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="17">
         <v>1792957</v>
       </c>
-      <c r="D46" s="36" t="s">
+      <c r="D46" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="E46" s="38">
-        <v>1</v>
-      </c>
-      <c r="F46" s="39">
-        <v>1.72</v>
-      </c>
-      <c r="G46" s="35">
+      <c r="E46" s="15">
+        <v>1</v>
+      </c>
+      <c r="F46" s="22">
+        <v>1.44</v>
+      </c>
+      <c r="G46" s="19">
         <f>E46*F46</f>
-        <v>1.72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="30" t="s">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B47" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="37" t="s">
+      <c r="B47" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="D47" s="36" t="s">
+      <c r="D47" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="E47" s="38">
+      <c r="E47" s="15">
         <v>2</v>
       </c>
-      <c r="F47" s="39">
-        <v>0.79</v>
-      </c>
-      <c r="G47" s="35">
+      <c r="F47" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="G47" s="19">
         <f t="shared" ref="G47:G48" si="2">E47*F47</f>
-        <v>1.58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="30" t="s">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B48" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="40" t="s">
+      <c r="B48" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D48" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E48" s="38">
-        <v>1</v>
-      </c>
-      <c r="F48" s="34">
-        <v>0.94</v>
-      </c>
-      <c r="G48" s="35">
+      <c r="E48" s="17">
+        <v>1</v>
+      </c>
+      <c r="F48" s="22">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="G48" s="19">
         <f t="shared" si="2"/>
-        <v>0.94</v>
+        <v>0.71499999999999997</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C49" s="9"/>
-      <c r="F49" s="17" t="s">
+      <c r="C49" s="8"/>
+      <c r="F49" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G49" s="26">
+      <c r="G49" s="23">
         <f>SUM(G3:G48)</f>
-        <v>80.175266666666658</v>
+        <v>70.89306666666667</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="26" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added link to motor module
</commit_message>
<xml_diff>
--- a/GoPack v2.0 - Pi 3 Simulink r2017b/GoPack Board Rev A/GoPack2 Parts List.xlsx
+++ b/GoPack v2.0 - Pi 3 Simulink r2017b/GoPack Board Rev A/GoPack2 Parts List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm_000\Desktop\RaspberryPIC Git\raspberry-pic-gopack\GoPack Board Rev A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm_000\Desktop\RaspberryPIC Git Test\raspberry-pic-gopack\GoPack v2.0 - Pi 3 Simulink r2017b\GoPack Board Rev A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D526418E-E63F-47E0-9493-C3DC085D2409}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4092936-3235-4B80-BD85-2C6B705A6009}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="300" windowWidth="20736" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="150">
   <si>
     <t>Item</t>
   </si>
@@ -468,6 +468,15 @@
   </si>
   <si>
     <t>9 Position Socket Connector 0.100" (2.54mm) Through Hole Gold</t>
+  </si>
+  <si>
+    <t>https://www.maxonmotor.com/maxon/view/product/control/4-Q-Servokontroller/438725</t>
+  </si>
+  <si>
+    <t>ESCON Module 50/5, 4-Q Servocontroller for DC/EC motors, 5/15 A, 10 - 50 VDC</t>
+  </si>
+  <si>
+    <t>The motor module that we have designed for is:</t>
   </si>
 </sst>
 </file>
@@ -1061,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2237,6 +2246,21 @@
         <v>107</v>
       </c>
     </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>

</xml_diff>